<commit_message>
training time captured, tsne iteration param included
</commit_message>
<xml_diff>
--- a/oclog/openset/notebooks/mytest.xlsx
+++ b/oclog/openset/notebooks/mytest.xlsx
@@ -14,7 +14,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="74">
+  <si>
+    <t>Unnamed: 0.1</t>
+  </si>
+  <si>
+    <t>Unnamed: 0</t>
+  </si>
   <si>
     <t>id</t>
   </si>
@@ -127,6 +133,9 @@
     <t>ptmodel_path</t>
   </si>
   <si>
+    <t>pt_time</t>
+  </si>
+  <si>
     <t>feature_from</t>
   </si>
   <si>
@@ -163,7 +172,28 @@
     <t>oc_optimizer</t>
   </si>
   <si>
-    <t>2022-04-26_20_15_56.052916_943a3d0dc56f11ecba05ac8247733f47</t>
+    <t>oc_tr_time</t>
+  </si>
+  <si>
+    <t>centroid_plot_start</t>
+  </si>
+  <si>
+    <t>total_oc_time</t>
+  </si>
+  <si>
+    <t>tsne_n_iter</t>
+  </si>
+  <si>
+    <t>tsne_perplexity</t>
+  </si>
+  <si>
+    <t>2022-04-27_06_53_57.955941_b60511fbc5c811ecba05ac8247733f47</t>
+  </si>
+  <si>
+    <t>2022-04-27_07_52_11.033363_d80e62c1c5d011ecba05ac8247733f47</t>
+  </si>
+  <si>
+    <t>2022-04-27_08_20_12.307190_c22c69a3c5d411eca8e1ac8247733f47</t>
   </si>
   <si>
     <t>C:\ML_data\Logs\BGL.log</t>
@@ -184,6 +214,9 @@
     <t>4.9835577,4.987583,5.033294,4.9719653,4.9852686</t>
   </si>
   <si>
+    <t>6.8490844,6.853139</t>
+  </si>
+  <si>
     <t>adam</t>
   </si>
   <si>
@@ -193,7 +226,13 @@
     <t>ptmodel</t>
   </si>
   <si>
-    <t>data\ptmodel_2022-04-26_20_13_05.488013/</t>
+    <t>data\ptmodel_2022-04-27_06_51_01.210878/</t>
+  </si>
+  <si>
+    <t>data\ptmodel_2022-04-27_07_49_27.544349/</t>
+  </si>
+  <si>
+    <t>data\ptmodel_2022-04-27_08_06_47.047017/</t>
   </si>
   <si>
     <t>train_data</t>
@@ -554,13 +593,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AX2"/>
+  <dimension ref="A1:BF4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:50">
+    <row r="1" spans="1:58">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -708,154 +747,533 @@
       <c r="AX1" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="AY1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="2" spans="1:50">
+    <row r="2" spans="1:58">
       <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>49</v>
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
       </c>
       <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2">
         <v>32</v>
       </c>
-      <c r="D2">
+      <c r="F2">
         <v>32</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>64</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K2" t="s">
+        <v>63</v>
+      </c>
+      <c r="L2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>0.8</v>
+      </c>
+      <c r="N2">
+        <v>500</v>
+      </c>
+      <c r="O2" t="s">
+        <v>64</v>
+      </c>
+      <c r="P2">
+        <v>5</v>
+      </c>
+      <c r="Q2" t="b">
+        <v>1</v>
+      </c>
+      <c r="R2" t="b">
+        <v>1</v>
+      </c>
+      <c r="S2" t="b">
+        <v>1</v>
+      </c>
+      <c r="T2" t="b">
+        <v>1</v>
+      </c>
+      <c r="U2" t="b">
+        <v>1</v>
+      </c>
+      <c r="V2" t="b">
+        <v>1</v>
+      </c>
+      <c r="W2" t="s">
+        <v>65</v>
+      </c>
+      <c r="X2">
+        <v>278.4970092773438</v>
+      </c>
+      <c r="Y2">
+        <v>0.7935053703064504</v>
+      </c>
+      <c r="Z2">
+        <v>0.5880684190574047</v>
+      </c>
+      <c r="AA2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB2">
         <v>50</v>
       </c>
-      <c r="G2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I2" t="s">
-        <v>53</v>
-      </c>
-      <c r="J2" t="b">
-        <v>1</v>
-      </c>
-      <c r="K2">
+      <c r="AC2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD2">
+        <v>5</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AG2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH2">
+        <v>6</v>
+      </c>
+      <c r="AI2">
+        <v>10</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AL2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM2">
+        <v>3</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AO2">
+        <v>40.39199113845825</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AQ2">
+        <v>48.853</v>
+      </c>
+      <c r="AR2">
+        <v>0</v>
+      </c>
+      <c r="AS2">
+        <v>0.4859436025389964</v>
+      </c>
+      <c r="AT2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AU2">
+        <v>0.4097222222222222</v>
+      </c>
+      <c r="AV2">
+        <v>40.97</v>
+      </c>
+      <c r="AW2">
+        <v>7</v>
+      </c>
+      <c r="AX2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AY2">
+        <v>3</v>
+      </c>
+      <c r="AZ2">
+        <v>2</v>
+      </c>
+      <c r="BB2">
+        <v>173.7197544574738</v>
+      </c>
+      <c r="BC2">
+        <v>1651022637.95694</v>
+      </c>
+      <c r="BD2">
+        <v>177.4426748752594</v>
+      </c>
+    </row>
+    <row r="3" spans="1:58">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3">
+        <v>32</v>
+      </c>
+      <c r="F3">
+        <v>32</v>
+      </c>
+      <c r="G3">
+        <v>64</v>
+      </c>
+      <c r="H3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" t="s">
+        <v>62</v>
+      </c>
+      <c r="K3" t="s">
+        <v>63</v>
+      </c>
+      <c r="L3" t="b">
+        <v>1</v>
+      </c>
+      <c r="M3">
         <v>0.8</v>
       </c>
-      <c r="L2">
+      <c r="N3">
         <v>500</v>
       </c>
-      <c r="M2" t="s">
-        <v>54</v>
-      </c>
-      <c r="N2">
+      <c r="O3" t="s">
+        <v>64</v>
+      </c>
+      <c r="P3">
         <v>5</v>
       </c>
-      <c r="O2" t="b">
-        <v>1</v>
-      </c>
-      <c r="P2" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q2" t="b">
-        <v>1</v>
-      </c>
-      <c r="R2" t="b">
-        <v>1</v>
-      </c>
-      <c r="S2" t="b">
-        <v>1</v>
-      </c>
-      <c r="T2" t="b">
-        <v>1</v>
-      </c>
-      <c r="U2" t="s">
-        <v>55</v>
-      </c>
-      <c r="V2">
+      <c r="Q3" t="b">
+        <v>1</v>
+      </c>
+      <c r="R3" t="b">
+        <v>1</v>
+      </c>
+      <c r="S3" t="b">
+        <v>1</v>
+      </c>
+      <c r="T3" t="b">
+        <v>1</v>
+      </c>
+      <c r="U3" t="b">
+        <v>1</v>
+      </c>
+      <c r="V3" t="b">
+        <v>1</v>
+      </c>
+      <c r="W3" t="s">
+        <v>65</v>
+      </c>
+      <c r="X3">
         <v>278.4970092773438</v>
       </c>
-      <c r="W2">
+      <c r="Y3">
         <v>0.7935053703064504</v>
       </c>
-      <c r="X2">
+      <c r="Z3">
         <v>0.5880684190574047</v>
       </c>
-      <c r="Y2" t="b">
+      <c r="AA3" t="b">
         <v>0</v>
       </c>
-      <c r="Z2">
+      <c r="AB3">
         <v>50</v>
       </c>
-      <c r="AA2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AB2">
+      <c r="AC3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD3">
         <v>5</v>
       </c>
-      <c r="AC2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD2" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE2" t="b">
-        <v>1</v>
-      </c>
-      <c r="AF2">
+      <c r="AE3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AG3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH3">
         <v>6</v>
       </c>
-      <c r="AG2">
+      <c r="AI3">
         <v>10</v>
       </c>
-      <c r="AH2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AJ2" t="b">
-        <v>1</v>
-      </c>
-      <c r="AK2">
+      <c r="AJ3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AL3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM3">
         <v>3</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AN3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO3">
+        <v>39.82676148414612</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AQ3">
+        <v>48.853</v>
+      </c>
+      <c r="AR3">
+        <v>0</v>
+      </c>
+      <c r="AS3">
+        <v>0.4859436025389964</v>
+      </c>
+      <c r="AT3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AU3">
+        <v>0.4097222222222222</v>
+      </c>
+      <c r="AV3">
+        <v>40.97</v>
+      </c>
+      <c r="AW3">
+        <v>7</v>
+      </c>
+      <c r="AX3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AY3">
+        <v>3</v>
+      </c>
+      <c r="AZ3">
+        <v>2</v>
+      </c>
+      <c r="BB3">
+        <v>160.5271420478821</v>
+      </c>
+      <c r="BC3">
+        <v>1651026131.033363</v>
+      </c>
+      <c r="BD3">
+        <v>164.7280344963074</v>
+      </c>
+      <c r="BE3">
+        <v>2000</v>
+      </c>
+      <c r="BF3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:58">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
         <v>59</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="E4">
+        <v>32</v>
+      </c>
+      <c r="F4">
+        <v>32</v>
+      </c>
+      <c r="G4">
+        <v>64</v>
+      </c>
+      <c r="H4" t="s">
         <v>60</v>
       </c>
-      <c r="AN2">
-        <v>48.853</v>
-      </c>
-      <c r="AO2">
+      <c r="I4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K4" t="s">
+        <v>63</v>
+      </c>
+      <c r="L4" t="b">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>0.8</v>
+      </c>
+      <c r="N4">
+        <v>5000</v>
+      </c>
+      <c r="O4" t="s">
+        <v>64</v>
+      </c>
+      <c r="P4">
+        <v>5</v>
+      </c>
+      <c r="Q4" t="b">
+        <v>1</v>
+      </c>
+      <c r="R4" t="b">
+        <v>1</v>
+      </c>
+      <c r="S4" t="b">
+        <v>1</v>
+      </c>
+      <c r="T4" t="b">
+        <v>1</v>
+      </c>
+      <c r="U4" t="b">
+        <v>1</v>
+      </c>
+      <c r="V4" t="b">
+        <v>1</v>
+      </c>
+      <c r="W4" t="s">
+        <v>66</v>
+      </c>
+      <c r="X4">
+        <v>1318.860229492188</v>
+      </c>
+      <c r="Y4">
+        <v>0.9542974079126875</v>
+      </c>
+      <c r="Z4">
+        <v>0.9979756753212693</v>
+      </c>
+      <c r="AA4" t="b">
         <v>0</v>
       </c>
-      <c r="AP2">
-        <v>0.4859436025389964</v>
-      </c>
-      <c r="AQ2" t="b">
+      <c r="AB4">
+        <v>50</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD4">
+        <v>2</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AG4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH4">
+        <v>6</v>
+      </c>
+      <c r="AI4">
+        <v>50</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AL4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM4">
+        <v>3</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO4">
+        <v>97.81152153015137</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AQ4">
+        <v>66.66670000000001</v>
+      </c>
+      <c r="AR4">
         <v>0</v>
       </c>
-      <c r="AR2">
-        <v>0.4097222222222222</v>
-      </c>
-      <c r="AS2">
-        <v>40.97</v>
-      </c>
-      <c r="AT2">
+      <c r="AS4">
+        <v>0.8585069444444444</v>
+      </c>
+      <c r="AT4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AU4">
+        <v>0.8585069444444443</v>
+      </c>
+      <c r="AV4">
+        <v>85.84999999999999</v>
+      </c>
+      <c r="AW4">
         <v>7</v>
       </c>
-      <c r="AU2" t="b">
-        <v>1</v>
-      </c>
-      <c r="AV2">
+      <c r="AX4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AY4">
         <v>3</v>
       </c>
-      <c r="AW2">
+      <c r="AZ4">
         <v>2</v>
+      </c>
+      <c r="BB4">
+        <v>794.5880978107452</v>
+      </c>
+      <c r="BC4">
+        <v>1651027812.30719</v>
+      </c>
+      <c r="BD4">
+        <v>808.3329162597656</v>
+      </c>
+      <c r="BE4">
+        <v>2000</v>
+      </c>
+      <c r="BF4">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>